<commit_message>
condición en caso de no tener campo a vincular
</commit_message>
<xml_diff>
--- a/importador/xls/agrupaciones.xlsx
+++ b/importador/xls/agrupaciones.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">familia_id</t>
   </si>
   <si>
+    <t xml:space="preserve">transcripcionFonetica</t>
+  </si>
+  <si>
     <t xml:space="preserve">comunidades</t>
   </si>
   <si>
@@ -85,85 +88,100 @@
     <t xml:space="preserve">normaDeEscritura</t>
   </si>
   <si>
-    <t xml:space="preserve">NomOri 1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomCast 1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,2,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomOri 1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomCast 1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,5,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomOri 1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomCast 1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,8,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomOri 2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomCast 2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,11,12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomOri 2.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomCast 2.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,14,15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomOri 2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomCast 2.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16,17,18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomOri 3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomCast 3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19,20,21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomOri 3.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomCast 3.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22,23,24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomOri 3.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NomCast 3.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25,26,27</t>
+    <t xml:space="preserve">Bot’una</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matlatzinca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chatino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chinanteco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dibaku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuicateco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hñäñu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otomí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jñartjo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mazahua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nahuatl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nahua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mexicano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nayeeri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odami</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tepehuano del norte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O’dam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tepehuano del sur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oichkama no’oka/oishkam no’ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O’otam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pápago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ralámuli raicha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarahumara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wixárika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huichol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yoremnokki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kickapoo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kikapú</t>
   </si>
 </sst>
 </file>
@@ -265,37 +283,38 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="28.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="21.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="25.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="26.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="20.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="28.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="21.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="25.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -359,18 +378,18 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="0" t="s">
         <v>23</v>
       </c>
       <c r="F2" s="0" t="n">
@@ -385,10 +404,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>1</v>
@@ -399,13 +415,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>1</v>
@@ -416,16 +429,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -433,16 +443,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -450,16 +460,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -467,16 +474,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>41</v>
+        <v>34</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>35</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -484,16 +491,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -501,15 +505,110 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="F13" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="C14" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F14" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="0" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>